<commit_message>
1. skip merged item; 2. check overlap inside the RACk
</commit_message>
<xml_diff>
--- a/dailywork/RackDrawer/testdata/IDCv2.xlsx
+++ b/dailywork/RackDrawer/testdata/IDCv2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F3E0B43A-C0E7-4CE8-A293-CCFF9C0965BA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{772919A7-DC65-40FE-B923-54E7A035A720}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3345" yWindow="1395" windowWidth="15660" windowHeight="7395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3117" uniqueCount="1662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="1661">
   <si>
     <t>机柜位</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6208,10 +6208,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4-6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2-3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6428,8 +6424,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>汇总条目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>汇总记录</t>
   </si>
 </sst>
 </file>
@@ -6947,8 +6942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="E306" sqref="E306"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8733,7 +8728,9 @@
       <c r="H69" s="15">
         <v>43273</v>
       </c>
-      <c r="I69" s="14"/>
+      <c r="I69" s="14" t="s">
+        <v>1660</v>
+      </c>
     </row>
     <row r="70" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="12" t="s">
@@ -8764,7 +8761,7 @@
         <v>84</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>1606</v>
+        <v>1611</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>1603</v>
@@ -8785,7 +8782,7 @@
         <v>84</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="D72" s="14" t="s">
         <v>1603</v>
@@ -9535,7 +9532,7 @@
         <v>127</v>
       </c>
       <c r="C100" s="13" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="D100" s="14" t="s">
         <v>139</v>
@@ -9544,30 +9541,32 @@
         <v>140</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="G100" s="13"/>
       <c r="H100" s="15">
         <v>43273</v>
       </c>
-      <c r="I100" s="14"/>
+      <c r="I100" s="14" t="s">
+        <v>1660</v>
+      </c>
     </row>
     <row r="101" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="12" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="B101" s="12" t="s">
         <v>127</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="D101" s="14" t="s">
         <v>74</v>
       </c>
       <c r="E101" s="14"/>
       <c r="F101" s="14" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="G101" s="13"/>
       <c r="H101" s="15">
@@ -9577,20 +9576,20 @@
     </row>
     <row r="102" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="12" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="B102" s="12" t="s">
         <v>127</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="D102" s="14" t="s">
         <v>74</v>
       </c>
       <c r="E102" s="14"/>
       <c r="F102" s="14" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="G102" s="13"/>
       <c r="H102" s="15">
@@ -9600,20 +9599,20 @@
     </row>
     <row r="103" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="12" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="B103" s="12" t="s">
         <v>127</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="D103" s="14" t="s">
         <v>74</v>
       </c>
       <c r="E103" s="14"/>
       <c r="F103" s="14" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="G103" s="13"/>
       <c r="H103" s="15">
@@ -9623,20 +9622,20 @@
     </row>
     <row r="104" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="12" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="B104" s="12" t="s">
         <v>127</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="D104" s="14" t="s">
         <v>74</v>
       </c>
       <c r="E104" s="14"/>
       <c r="F104" s="14" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="G104" s="13"/>
       <c r="H104" s="15">
@@ -9646,20 +9645,20 @@
     </row>
     <row r="105" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="12" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="B105" s="12" t="s">
         <v>127</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="D105" s="14" t="s">
         <v>74</v>
       </c>
       <c r="E105" s="14"/>
       <c r="F105" s="14" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="G105" s="13"/>
       <c r="H105" s="15">
@@ -14024,23 +14023,25 @@
         <v>290</v>
       </c>
       <c r="F272" s="14" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="G272" s="13"/>
       <c r="H272" s="15">
         <v>43278</v>
       </c>
-      <c r="I272" s="14"/>
+      <c r="I272" s="14" t="s">
+        <v>1660</v>
+      </c>
     </row>
     <row r="273" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A273" s="12" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="B273" s="12" t="s">
         <v>272</v>
       </c>
       <c r="C273" s="13" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="D273" s="14" t="s">
         <v>74</v>
@@ -14049,7 +14050,7 @@
         <v>290</v>
       </c>
       <c r="F273" s="14" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="G273" s="13"/>
       <c r="H273" s="15">
@@ -14059,13 +14060,13 @@
     </row>
     <row r="274" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A274" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B274" s="12" t="s">
         <v>272</v>
       </c>
       <c r="C274" s="13" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="D274" s="14" t="s">
         <v>74</v>
@@ -14074,7 +14075,7 @@
         <v>290</v>
       </c>
       <c r="F274" s="14" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="G274" s="13"/>
       <c r="H274" s="15">
@@ -14084,13 +14085,13 @@
     </row>
     <row r="275" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A275" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B275" s="12" t="s">
         <v>272</v>
       </c>
       <c r="C275" s="13" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="D275" s="14" t="s">
         <v>74</v>
@@ -14099,7 +14100,7 @@
         <v>290</v>
       </c>
       <c r="F275" s="14" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="G275" s="13"/>
       <c r="H275" s="15">
@@ -14394,14 +14395,14 @@
         <v>1582</v>
       </c>
       <c r="F286" s="14" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="G286" s="13"/>
       <c r="H286" s="15">
         <v>43287</v>
       </c>
       <c r="I286" s="14" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="287" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14421,7 +14422,7 @@
         <v>1581</v>
       </c>
       <c r="F287" s="14" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="G287" s="13"/>
       <c r="H287" s="15">
@@ -14446,7 +14447,7 @@
         <v>1583</v>
       </c>
       <c r="F288" s="14" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="G288" s="13"/>
       <c r="H288" s="15">
@@ -14478,7 +14479,7 @@
         <v>43287</v>
       </c>
       <c r="I289" s="14" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="290" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14498,14 +14499,14 @@
         <v>1587</v>
       </c>
       <c r="F290" s="14" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="G290" s="13"/>
       <c r="H290" s="15">
         <v>43287</v>
       </c>
       <c r="I290" s="14" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="291" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14525,14 +14526,14 @@
         <v>1587</v>
       </c>
       <c r="F291" s="14" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="G291" s="13"/>
       <c r="H291" s="15">
         <v>43287</v>
       </c>
       <c r="I291" s="14" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="292" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14552,14 +14553,14 @@
         <v>1589</v>
       </c>
       <c r="F292" s="14" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="G292" s="13"/>
       <c r="H292" s="15">
         <v>43287</v>
       </c>
       <c r="I292" s="14" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="293" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14579,7 +14580,7 @@
         <v>1590</v>
       </c>
       <c r="F293" s="14" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="G293" s="13"/>
       <c r="H293" s="15">
@@ -14589,22 +14590,22 @@
     </row>
     <row r="294" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A294" s="12" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="B294" s="12" t="s">
         <v>1571</v>
       </c>
       <c r="C294" s="13" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="D294" s="14" t="s">
+        <v>1657</v>
+      </c>
+      <c r="E294" s="14" t="s">
         <v>1658</v>
       </c>
-      <c r="E294" s="14" t="s">
+      <c r="F294" s="14" t="s">
         <v>1659</v>
-      </c>
-      <c r="F294" s="14" t="s">
-        <v>1660</v>
       </c>
       <c r="G294" s="13"/>
       <c r="H294" s="15">
@@ -14629,7 +14630,7 @@
         <v>1592</v>
       </c>
       <c r="F295" s="14" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="G295" s="13"/>
       <c r="H295" s="15">
@@ -14654,7 +14655,7 @@
         <v>1594</v>
       </c>
       <c r="F296" s="14" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="G296" s="13"/>
       <c r="H296" s="15">
@@ -14793,17 +14794,19 @@
       <c r="H301" s="15">
         <v>43278</v>
       </c>
-      <c r="I301" s="14"/>
+      <c r="I301" s="14" t="s">
+        <v>1660</v>
+      </c>
     </row>
     <row r="302" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A302" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B302" s="12" t="s">
         <v>314</v>
       </c>
       <c r="C302" s="13" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D302" s="14" t="s">
         <v>15</v>
@@ -14820,13 +14823,13 @@
     </row>
     <row r="303" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A303" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B303" s="12" t="s">
         <v>314</v>
       </c>
       <c r="C303" s="13" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="D303" s="14" t="s">
         <v>15</v>
@@ -14843,13 +14846,13 @@
     </row>
     <row r="304" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A304" s="12" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="B304" s="12" t="s">
         <v>314</v>
       </c>
       <c r="C304" s="13" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D304" s="14" t="s">
         <v>15</v>
@@ -14970,7 +14973,7 @@
     </row>
     <row r="309" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A309" s="12" t="s">
-        <v>1661</v>
+        <v>78</v>
       </c>
       <c r="B309" s="12" t="s">
         <v>515</v>
@@ -14993,17 +14996,19 @@
       <c r="H309" s="15">
         <v>43278</v>
       </c>
-      <c r="I309" s="14"/>
+      <c r="I309" s="14" t="s">
+        <v>1660</v>
+      </c>
     </row>
     <row r="310" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A310" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B310" s="12" t="s">
         <v>515</v>
       </c>
       <c r="C310" s="13" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="D310" s="14" t="s">
         <v>15</v>
@@ -15020,13 +15025,13 @@
     </row>
     <row r="311" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A311" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B311" s="12" t="s">
         <v>515</v>
       </c>
       <c r="C311" s="13" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="D311" s="14" t="s">
         <v>15</v>
@@ -15043,13 +15048,13 @@
     </row>
     <row r="312" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A312" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B312" s="12" t="s">
         <v>515</v>
       </c>
       <c r="C312" s="13" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="D312" s="14" t="s">
         <v>15</v>
@@ -15066,13 +15071,13 @@
     </row>
     <row r="313" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A313" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B313" s="12" t="s">
         <v>515</v>
       </c>
       <c r="C313" s="13" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="D313" s="14" t="s">
         <v>15</v>
@@ -15089,19 +15094,19 @@
     </row>
     <row r="314" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A314" s="12" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="B314" s="12" t="s">
         <v>515</v>
       </c>
       <c r="C314" s="13" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="D314" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E314" s="14" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="F314" s="14"/>
       <c r="G314" s="13"/>
@@ -15112,19 +15117,19 @@
     </row>
     <row r="315" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A315" s="12" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="B315" s="12" t="s">
         <v>515</v>
       </c>
       <c r="C315" s="13" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="D315" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E315" s="14" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="F315" s="14"/>
       <c r="G315" s="13"/>
@@ -15135,13 +15140,13 @@
     </row>
     <row r="316" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A316" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B316" s="12" t="s">
         <v>515</v>
       </c>
       <c r="C316" s="13" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="D316" s="14" t="s">
         <v>15</v>
@@ -15158,13 +15163,13 @@
     </row>
     <row r="317" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A317" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B317" s="12" t="s">
         <v>515</v>
       </c>
       <c r="C317" s="13" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="D317" s="14" t="s">
         <v>15</v>
@@ -15181,13 +15186,13 @@
     </row>
     <row r="318" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A318" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B318" s="12" t="s">
         <v>515</v>
       </c>
       <c r="C318" s="13" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="D318" s="14" t="s">
         <v>15</v>
@@ -15204,7 +15209,7 @@
     </row>
     <row r="319" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A319" s="12" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B319" s="12" t="s">
         <v>515</v>

</xml_diff>